<commit_message>
SoE excel file edited
</commit_message>
<xml_diff>
--- a/data/soe_tables_20240205.xlsx
+++ b/data/soe_tables_20240205.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoe-my.sharepoint.com/personal/mmacleo2_ed_ac_uk/Documents/Applications/WT Mental Health/LSR3/test020224/LSR3/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/FS/HomeDrives/vc18e501/ESM/GALENOS - WP2/WP2/LSR3/LSR3_taar1_A/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{8B376FA9-C458-48A9-A9AE-89173CAAB48E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1811E55-DE35-0B4A-B1DC-B3E4B469A95A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{5B3852FF-2BEC-B94D-907F-9BD79E8D9C2A}"/>
+    <workbookView xWindow="4520" yWindow="500" windowWidth="24280" windowHeight="17500" activeTab="1" xr2:uid="{5B3852FF-2BEC-B94D-907F-9BD79E8D9C2A}"/>
   </bookViews>
   <sheets>
     <sheet name="TvC" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="62">
   <si>
     <t>Outcome</t>
   </si>
@@ -62,40 +62,6 @@
     <t>Cognition</t>
   </si>
   <si>
-    <t>3 experimental comparisons from 1 experiment in 1 publications involving 1 animal strains and reporting data from 36 animals; insufficient data for further analysis</t>
-  </si>
-  <si>
-    <t>No other risks identified</t>
-  </si>
-  <si>
-    <t>19 experimental comparisons from 5 experiments in 4 publications involving 4 animal strains and reporting data from 312 animals; SMD =0.8 (95% CI: -0.301 to 1.9); (95% PrI -1.609 to 3.208) (Section 2.2.3)
-No significant heterogeneity was observed (Section 2.2.4)
-Drug effects: there was no significant modifying effect of drug selectivity, potency, dose or standardised dose (Figs 2.2.4.5 through 2.2.4.7)</t>
-  </si>
-  <si>
-    <t>Moderate risk of bias likely to exaggerate the effects of TAAR1 agonists.
-All studies had unclear risk of bias for most of the SyRCLE items
-Reporting was mostly incomplete; the median number of ARRIVE items reported was 13 (of 23)</t>
-  </si>
-  <si>
-    <t>Moderate risk of bias likely to exaggerate the effects of TAAR1 agonists.
-All studies had unclear risk of bias for most of the SyRCLE items
-Reporting was mostly incomplete; the median number of ARRIVE items reported was 15 (of 23)</t>
-  </si>
-  <si>
-    <t>Moderate risk of bias likely to exaggerate the effects of TAAR1 agonists.
-No studies preregistered their analyses; 
-There was no evidence for small study effects (Section 2.2.6)</t>
-  </si>
-  <si>
-    <t>The included study was at unclear risk of bias (SyRCLE); the  number of ARRIVE items reported was 16 (of 23)</t>
-  </si>
-  <si>
-    <t>Moderate risk of bias likely to exaggerate the effects of TAAR1 agonists.
-No studies preregistered their analyses
-Evidence for small study effects not saught</t>
-  </si>
-  <si>
     <t>Homological validity</t>
   </si>
   <si>
@@ -201,15 +167,6 @@
     <t>Dimension</t>
   </si>
   <si>
-    <t>Moderate risk of bias likely to exaggerate the effects of TAAR1 agonists.
-No studies preregistered their analyses; 
-There was significant evidence for small study effects (Section 2.1.6)</t>
-  </si>
-  <si>
-    <t>21 experimental comparisons from 39 experiments in 4 publications involving 7 animal strains and reporting data from 336 animals; SMD =-0.622 (95% CI: -1.324 to 0.08): (95% PrI  -2.272 to 1.029)
-(non significantly favours conventional antipsychotics); Dose effects: insufficient data</t>
-  </si>
-  <si>
     <t>~</t>
   </si>
   <si>
@@ -219,32 +176,59 @@
     <t>Pharmacological models (psychostimulant models (cocaine, amphetamine etc), NMDA models (phencyclidine, MK801 etc))</t>
   </si>
   <si>
-    <t>125 experimental comparisons from 39 experiments in 13 publications involving 8 animal strains and reporting data from 1945 animals; SMD = 1.032 (95% C to .751 to 1.313); (95% PrI 0.008 to 2.056) (Section 2.1.3)
-No significant heterogeneity was observed (Section 2.1.4)
-Drug effects: there was no significant modifying effect of drug selectivity, potency, or dose (Figs 2.1.4.8 through 2.1.4.9) but there was a relationship with standardised dose (Fig 2.1.4.10)</t>
-  </si>
-  <si>
-    <t>Moderate risk of indirectness
-For explanation, see [1] below</t>
-  </si>
-  <si>
-    <t>Moderate risk of indirectness
-For explanation, see [2] below</t>
-  </si>
-  <si>
-    <t>Moderate risk of indirectness
-For explanation, see [3] below</t>
-  </si>
-  <si>
-    <t>Moderate risk of indirectness
-For explanation, see [4] below</t>
+    <t>Moderate risk of bias likely to exaggerate the effects of TAAR1 agonists. All studies had unclear risk of bias for most of the SyRCLE items. Reporting was mostly incomplete; the median number of ARRIVE items reported was 13 (of 22).</t>
+  </si>
+  <si>
+    <t>Moderate risk of bias likely to exaggerate the effects of TAAR1 agonists. No studies preregistered their analyses. There was evidence of small-study effects (Section 2.1.6).</t>
+  </si>
+  <si>
+    <t>Moderate risk of indirectness. For explanation, see [1] below.</t>
+  </si>
+  <si>
+    <t>No other risks identified.</t>
+  </si>
+  <si>
+    <t>Moderate risk of indirectness. For explanation, see [2] below.</t>
+  </si>
+  <si>
+    <t>Moderate risk of bias likely to exaggerate the effects of TAAR1 agonists. No studies preregistered their analyses. There was no evidence of small-study effects (Section 2.2.6).</t>
+  </si>
+  <si>
+    <t>Moderate risk of bias likely to exaggerate the effects of TAAR1 agonists. All studies had unclear risk of bias for most of the SyRCLE items. Reporting was mostly incomplete; the median number of ARRIVE items reported was 15 (of 22).</t>
+  </si>
+  <si>
+    <t>19 experimental comparisons from 5 experiments in 4 publications involving 4 animal strains and reporting data from 312 animals; SMD =0.8 (95% CI: -0.301 to 1.9; 95% PrI -1.609 to 3.208) (Section 2.2.3). No significant heterogeneity was observed. Drug effects: there was no significant modifying effect of drug selectivity, potency, dose or standardised dose (Section 2.2.4).</t>
+  </si>
+  <si>
+    <t>128 experimental comparisons from 42 experiments in 13 publications involving 9 animal strains and reporting data from 1945 animals; SMD = 0.973 (95% CI to .582 to 1.364; 95% PrI -0.308 to 2.254) (Section 2.1.3). Some heterogeneity was observed; Drug effects: there was no significant modifying effect of drug selectivity, potency, or dose (Section 2.1.4) but there was a relationship with standardised dose (Fig 2.1.4.10).</t>
+  </si>
+  <si>
+    <t>21 experimental comparisons from 7 experiments in 4 publications involving 2 animal strains and reporting data from 336 animals; SMD =-0.622 (95% CI: -1.324 to 0.08; 95% PrI  -2.272 to 1.029). Dose effects: insufficient data.</t>
+  </si>
+  <si>
+    <t>Moderate risk of bias likely to exaggerate the effects of TAAR1 agonists. No studies preregistered their analyses. Evidence for small-study effects not saught.</t>
+  </si>
+  <si>
+    <t>Moderate risk of indirectness. For explanation, see [3] below.</t>
+  </si>
+  <si>
+    <t>Moderate risk of indirectness. For explanation, see [4] below.</t>
+  </si>
+  <si>
+    <t>3 experimental comparisons from 1 experiment in 1 publications involving 1 animal strains and reporting data from 36 animals; insufficient data for further analysis.</t>
+  </si>
+  <si>
+    <t>The included study was at unclear risk of bias (SyRCLE); the number of ARRIVE items reported was 16 (of 22).</t>
+  </si>
+  <si>
+    <t>Moderate risk of bias likely to exaggerate the effects of TAAR1 agonists. The study did not preregistered its analyses.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -375,7 +359,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -389,11 +373,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -424,9 +405,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -774,17 +752,17 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView topLeftCell="B3" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" style="3" customWidth="1"/>
-    <col min="2" max="2" width="21.109375" style="3" customWidth="1"/>
-    <col min="3" max="16384" width="11.5546875" style="3"/>
+    <col min="2" max="2" width="21.1640625" style="3" customWidth="1"/>
+    <col min="3" max="16384" width="11.5" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="26.25" thickBot="1">
+    <row r="1" spans="1:6" ht="43" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -804,47 +782,47 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="249.75" customHeight="1" thickBot="1">
+    <row r="2" spans="1:6" ht="249.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="248.25" customHeight="1" thickBot="1">
+      <c r="B2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="248.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="6" customFormat="1">
+      <c r="B3" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -852,7 +830,7 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" s="6" customFormat="1">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -860,7 +838,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" s="6" customFormat="1">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -868,8 +846,8 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="7"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -880,17 +858,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2502A7F1-62AA-1544-B3B9-07F305A4B185}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" style="3" customWidth="1"/>
-    <col min="2" max="16384" width="11.5546875" style="3"/>
+    <col min="2" max="16384" width="11.5" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="26.25" thickBot="1">
+    <row r="1" spans="1:6" ht="43" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -910,47 +888,47 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="268.5" thickBot="1">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:6" ht="307" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="8" t="s">
+      <c r="B2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="239" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="179.25" thickBot="1">
-      <c r="A3" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="6" customFormat="1">
+      <c r="D3" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -958,7 +936,7 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" s="6" customFormat="1">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -966,7 +944,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" s="6" customFormat="1">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -974,7 +952,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" s="6" customFormat="1">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -982,7 +960,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" s="6" customFormat="1">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -1003,265 +981,265 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="12"/>
-    <col min="2" max="2" width="14" style="12" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="12"/>
+    <col min="1" max="1" width="8.83203125" style="11"/>
+    <col min="2" max="2" width="14" style="11" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="26.25" thickBot="1">
-      <c r="A1" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="11" t="s">
+    <row r="1" spans="1:10" ht="29" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="86.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="B2" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="D2" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="155" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="B3" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="C3" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="D3" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="F3" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="G3" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="176.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="86.25" customHeight="1" thickBot="1">
-      <c r="A2" s="13" t="s">
+      <c r="E4" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="13" t="s">
+      <c r="F4" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="115.5" thickBot="1">
-      <c r="A3" s="15" t="s">
+      <c r="G4" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="H4" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="I4" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="J4" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="409.6" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="J3" s="14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="176.25" customHeight="1" thickBot="1">
-      <c r="A4" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="10" t="s">
+    </row>
+    <row r="6" spans="1:10" ht="99" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="I6" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="18"/>
+    </row>
+    <row r="7" spans="1:10" ht="169" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="B7" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="I7" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="I4" s="10" t="s">
+    </row>
+    <row r="8" spans="1:10" ht="155" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="345" thickBot="1">
-      <c r="A5" s="17" t="s">
+      <c r="I8" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8" s="13" t="s">
         <v>37</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="I5" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="J5" s="19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="64.5" thickBot="1">
-      <c r="A6" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="J6" s="20"/>
-    </row>
-    <row r="7" spans="1:10" ht="102.75" thickBot="1">
-      <c r="A7" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="I7" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="J7" s="14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="102.75" thickBot="1">
-      <c r="A8" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="G8" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="I8" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="J8" s="14" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>